<commit_message>
Update model assets with corrected translations
</commit_message>
<xml_diff>
--- a/models/type3and5and10/AllModels.xlsx
+++ b/models/type3and5and10/AllModels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\pfHRP_MLModel\models\type3and5and10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558E322-0D06-4BCB-B201-6ABDCCFDEE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA47AC7-FE80-43B7-98DE-E957020D86A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21585" yWindow="1650" windowWidth="14325" windowHeight="8010" xr2:uid="{56B93907-60D1-8B42-B22A-F58A3AADB790}"/>
+    <workbookView xWindow="14475" yWindow="3600" windowWidth="14325" windowHeight="8010" xr2:uid="{56B93907-60D1-8B42-B22A-F58A3AADB790}"/>
   </bookViews>
   <sheets>
     <sheet name="pfHRP2_Types3and5and10" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
   <si>
     <t>VotingEnsemble</t>
   </si>
@@ -65,15 +65,9 @@
     <t>TruncatedSVDWrapper</t>
   </si>
   <si>
-    <t>PCA</t>
-  </si>
-  <si>
     <t>SGD</t>
   </si>
   <si>
-    <t>SparseNormalizer</t>
-  </si>
-  <si>
     <t>LogisticRegression</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
   </si>
   <si>
     <t>BernoulliNaiveBayes</t>
-  </si>
-  <si>
-    <t>DecisionTree</t>
   </si>
   <si>
     <t>XGBoostClassifier</t>
@@ -444,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D572B11-BCE1-874F-A955-E5F547514390}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -469,114 +460,114 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>0.86980000000000002</v>
+        <v>0.83816000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0.86836999999999998</v>
+        <v>0.83816000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.85170000000000001</v>
+        <v>0.83816000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.83816000000000002</v>
+        <v>0.83408000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -587,7 +578,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -598,10 +589,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>0.83408000000000004</v>
@@ -609,10 +600,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>0.83408000000000004</v>
@@ -620,10 +611,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>0.83408000000000004</v>
@@ -631,10 +622,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>0.83408000000000004</v>
@@ -642,524 +633,186 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18">
-        <v>0.83408000000000004</v>
+        <v>0.83265</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19">
-        <v>0.83408000000000004</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>0.83408000000000004</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>0.83408000000000004</v>
+        <v>0.82857000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>0.83408000000000004</v>
+        <v>0.79864000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>0.83408000000000004</v>
+        <v>0.79837000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>0.83</v>
+        <v>0.79837000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>0.83</v>
+        <v>0.79837000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>0.83</v>
+        <v>0.79740999999999995</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>0.83</v>
+        <v>0.79429000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>0.83</v>
+        <v>0.79429000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>0.83</v>
+        <v>0.79429000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>0.83</v>
+        <v>0.78856999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>0.81408000000000003</v>
+        <v>0.65551000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C32">
-        <v>0.81169999999999998</v>
+        <v>0.64680000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33">
-        <v>0.80245</v>
+        <v>0.48693999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <v>0.79837000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35">
-        <v>0.79837000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36">
-        <v>0.79837000000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37">
-        <v>0.79740999999999995</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <v>0.78856999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39">
-        <v>0.78856999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40">
-        <v>0.77429000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>0.69530999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42">
-        <v>0.64680000000000004</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43">
         <v>0.42857000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44">
-        <v>0.72074000000000005</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45">
-        <v>0.71638999999999997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46">
-        <v>0.71035999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47">
-        <v>0.70884000000000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48">
-        <v>0.70877000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49">
-        <v>0.70769000000000004</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50">
-        <v>0.70530999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51">
-        <v>0.70328000000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52">
-        <v>0.69594999999999996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53">
-        <v>0.69220999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54">
-        <v>0.68722000000000005</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55">
-        <v>0.67091000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56">
-        <v>0.64705000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57">
-        <v>0.62673000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58">
-        <v>0.61468999999999996</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59">
-        <v>0.61160000000000003</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60">
-        <v>0.59880999999999995</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61">
-        <v>0.59404999999999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62">
-        <v>0.59370999999999996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63">
-        <v>0.37714999999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64">
-        <v>0.37714999999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65">
-        <v>0.37714999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>